<commit_message>
Create button onli market + JSON + Exel
</commit_message>
<xml_diff>
--- a/market.xlsx
+++ b/market.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kareg\Desktop\DND\D&amp;D_4\События\Рынок\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kareg\Desktop\keregan.github.io\keregan.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11535" windowHeight="6855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11535" windowHeight="5565"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="152">
   <si>
     <t>Название товара</t>
   </si>
@@ -478,13 +478,25 @@
   </si>
   <si>
     <t>Дополнения к зельям</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>quantity_in_stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,6 +567,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="14">
@@ -649,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -681,27 +700,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,8 +712,32 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,7 +776,7 @@
         <xdr:cNvPr id="2" name="Rounded Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE5C99B9-7C2D-4F38-5AA4-2CF88C1AAA48}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE5C99B9-7C2D-4F38-5AA4-2CF88C1AAA48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1116,8 +1138,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:ED120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q81" workbookViewId="0">
-      <selection activeCell="AA112" sqref="X1:AA112"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AA113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,40 +1170,40 @@
       <c r="G1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="X1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z1">
-        <v>1</v>
-      </c>
-      <c r="AA1">
-        <v>20</v>
+      <c r="X1" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y1" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z1" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA1" s="38" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="A2" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="E2" s="2"/>
       <c r="G2" s="25">
         <f>SUM(E3:E120)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
       <c r="X2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y2" t="s">
         <v>5</v>
@@ -1190,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -1206,16 +1228,16 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Y3" t="s">
         <v>5</v>
       </c>
       <c r="Z3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA3">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -1231,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y4" t="s">
         <v>5</v>
@@ -1240,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="AA4">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -1256,16 +1278,16 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y5" t="s">
         <v>5</v>
       </c>
       <c r="Z5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA5">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -1281,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y6" t="s">
         <v>5</v>
@@ -1306,16 +1328,16 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y7" t="s">
         <v>5</v>
       </c>
       <c r="Z7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AA7">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -1331,16 +1353,16 @@
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y8" t="s">
         <v>5</v>
       </c>
       <c r="Z8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -1369,16 +1391,16 @@
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
       <c r="X9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y9" t="s">
         <v>5</v>
       </c>
       <c r="Z9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -1394,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y10" t="s">
         <v>5</v>
@@ -1403,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="AA10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -1419,16 +1441,16 @@
         <v>0</v>
       </c>
       <c r="X11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y11" t="s">
         <v>5</v>
       </c>
       <c r="Z11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA11">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
@@ -1444,13 +1466,13 @@
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y12" t="s">
         <v>5</v>
       </c>
       <c r="Z12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA12">
         <v>10</v>
@@ -1469,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="X13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Y13" t="s">
         <v>5</v>
@@ -1478,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="AA13">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -1494,13 +1516,13 @@
         <v>0</v>
       </c>
       <c r="X14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Y14" t="s">
         <v>5</v>
       </c>
       <c r="Z14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA14">
         <v>40</v>
@@ -1519,16 +1541,16 @@
         <v>0</v>
       </c>
       <c r="X15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y15" t="s">
         <v>5</v>
       </c>
       <c r="Z15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA15">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -1544,16 +1566,16 @@
         <v>0</v>
       </c>
       <c r="X16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Y16" t="s">
         <v>5</v>
       </c>
       <c r="Z16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AA16">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
@@ -1569,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="X17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y17" t="s">
         <v>5</v>
@@ -1578,7 +1600,7 @@
         <v>3</v>
       </c>
       <c r="AA17">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
@@ -1594,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y18" t="s">
         <v>5</v>
@@ -1603,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="AA18">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
@@ -1619,16 +1641,16 @@
         <v>0</v>
       </c>
       <c r="X19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y19" t="s">
         <v>5</v>
       </c>
       <c r="Z19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA19">
-        <v>200</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
@@ -1644,16 +1666,16 @@
         <v>0</v>
       </c>
       <c r="X20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y20" t="s">
         <v>5</v>
       </c>
       <c r="Z20">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="AA20">
-        <v>10</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
@@ -1669,16 +1691,16 @@
         <v>0</v>
       </c>
       <c r="X21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y21" t="s">
         <v>5</v>
       </c>
       <c r="Z21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AA21">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
@@ -1694,16 +1716,16 @@
         <v>0</v>
       </c>
       <c r="X22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Y22" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="Z22">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="AA22">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
@@ -1719,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="X23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y23" t="s">
         <v>27</v>
@@ -1728,30 +1750,30 @@
         <v>5</v>
       </c>
       <c r="AA23">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="E24" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X24" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="Y24" t="s">
         <v>27</v>
       </c>
       <c r="Z24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA24">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
@@ -1767,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="X25" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="Y25" t="s">
         <v>27</v>
@@ -1792,16 +1814,16 @@
         <v>0</v>
       </c>
       <c r="X26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y26" t="s">
         <v>27</v>
       </c>
       <c r="Z26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA26">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
@@ -1817,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="X27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y27" t="s">
         <v>27</v>
@@ -1826,7 +1848,7 @@
         <v>3</v>
       </c>
       <c r="AA27">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
@@ -1842,16 +1864,16 @@
         <v>0</v>
       </c>
       <c r="X28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y28" t="s">
         <v>27</v>
       </c>
       <c r="Z28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
@@ -1867,16 +1889,16 @@
         <v>0</v>
       </c>
       <c r="X29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y29" t="s">
         <v>27</v>
       </c>
       <c r="Z29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA29">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
@@ -1892,16 +1914,16 @@
         <v>0</v>
       </c>
       <c r="X30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y30" t="s">
         <v>27</v>
       </c>
       <c r="Z30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AA30">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
@@ -1917,16 +1939,16 @@
         <v>0</v>
       </c>
       <c r="X31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y31" t="s">
         <v>27</v>
       </c>
       <c r="Z31">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AA31">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
@@ -1942,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="X32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Y32" t="s">
         <v>27</v>
@@ -1951,7 +1973,7 @@
         <v>7</v>
       </c>
       <c r="AA32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
@@ -1967,13 +1989,13 @@
         <v>0</v>
       </c>
       <c r="X33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y33" t="s">
         <v>27</v>
       </c>
       <c r="Z33">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA33">
         <v>2</v>
@@ -1992,16 +2014,16 @@
         <v>0</v>
       </c>
       <c r="X34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y34" t="s">
         <v>27</v>
       </c>
       <c r="Z34">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AA34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
@@ -2017,16 +2039,16 @@
         <v>0</v>
       </c>
       <c r="X35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y35" t="s">
         <v>27</v>
       </c>
       <c r="Z35">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA35">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -2042,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="X36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y36" t="s">
         <v>27</v>
@@ -2051,7 +2073,7 @@
         <v>10</v>
       </c>
       <c r="AA36">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -2067,16 +2089,16 @@
         <v>0</v>
       </c>
       <c r="X37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y37" t="s">
         <v>27</v>
       </c>
       <c r="Z37">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AA37">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
@@ -2092,16 +2114,16 @@
         <v>0</v>
       </c>
       <c r="X38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y38" t="s">
         <v>27</v>
       </c>
       <c r="Z38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AA38">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
@@ -2117,16 +2139,16 @@
         <v>0</v>
       </c>
       <c r="X39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y39" t="s">
         <v>27</v>
       </c>
       <c r="Z39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA39">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -2142,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="X40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y40" t="s">
         <v>27</v>
@@ -2151,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="AA40">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -2167,16 +2189,16 @@
         <v>0</v>
       </c>
       <c r="X41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y41" t="s">
         <v>27</v>
       </c>
       <c r="Z41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA41">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -2192,16 +2214,16 @@
         <v>0</v>
       </c>
       <c r="X42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y42" t="s">
         <v>27</v>
       </c>
       <c r="Z42">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AA42">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
@@ -2217,16 +2239,16 @@
         <v>0</v>
       </c>
       <c r="X43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Y43" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="Z43">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AA43">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -2242,13 +2264,13 @@
         <v>0</v>
       </c>
       <c r="X44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y44" t="s">
         <v>49</v>
       </c>
       <c r="Z44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA44">
         <v>2</v>
@@ -2267,39 +2289,39 @@
         <v>0</v>
       </c>
       <c r="X45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y45" t="s">
         <v>49</v>
       </c>
       <c r="Z45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AA45">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
       <c r="E46" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y46" t="s">
         <v>49</v>
       </c>
       <c r="Z46">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="AA46">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
@@ -2315,16 +2337,16 @@
         <v>0</v>
       </c>
       <c r="X47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y47" t="s">
         <v>49</v>
       </c>
       <c r="Z47">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AA47">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
@@ -2340,16 +2362,16 @@
         <v>0</v>
       </c>
       <c r="X48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y48" t="s">
         <v>49</v>
       </c>
       <c r="Z48">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AA48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
@@ -2365,16 +2387,16 @@
         <v>0</v>
       </c>
       <c r="X49" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="Y49" t="s">
         <v>49</v>
       </c>
       <c r="Z49">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AA49">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
@@ -2390,16 +2412,16 @@
         <v>0</v>
       </c>
       <c r="X50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y50" t="s">
         <v>49</v>
       </c>
       <c r="Z50">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AA50">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
@@ -2415,16 +2437,16 @@
         <v>0</v>
       </c>
       <c r="X51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y51" t="s">
         <v>49</v>
       </c>
       <c r="Z51">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AA51">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
@@ -2440,16 +2462,16 @@
         <v>0</v>
       </c>
       <c r="X52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Y52" t="s">
         <v>49</v>
       </c>
       <c r="Z52">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="AA52">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
@@ -2465,13 +2487,13 @@
         <v>0</v>
       </c>
       <c r="X53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Y53" t="s">
         <v>49</v>
       </c>
       <c r="Z53">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="AA53">
         <v>4</v>
@@ -2490,16 +2512,16 @@
         <v>0</v>
       </c>
       <c r="X54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y54" t="s">
         <v>49</v>
       </c>
       <c r="Z54">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AA54">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
@@ -2515,16 +2537,16 @@
         <v>0</v>
       </c>
       <c r="X55" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="Y55" t="s">
         <v>49</v>
       </c>
       <c r="Z55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AA55">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
@@ -2540,16 +2562,16 @@
         <v>0</v>
       </c>
       <c r="X56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y56" t="s">
         <v>49</v>
       </c>
       <c r="Z56">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA56">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -2565,16 +2587,16 @@
         <v>0</v>
       </c>
       <c r="X57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y57" t="s">
         <v>49</v>
       </c>
       <c r="Z57">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="AA57">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
@@ -2590,13 +2612,13 @@
         <v>0</v>
       </c>
       <c r="X58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y58" t="s">
         <v>49</v>
       </c>
       <c r="Z58">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="AA58">
         <v>3</v>
@@ -2615,16 +2637,16 @@
         <v>0</v>
       </c>
       <c r="X59" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="Y59" t="s">
         <v>49</v>
       </c>
       <c r="Z59">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AA59">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
@@ -2640,16 +2662,16 @@
         <v>0</v>
       </c>
       <c r="X60" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="Y60" t="s">
         <v>49</v>
       </c>
       <c r="Z60">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AA60">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
@@ -2665,16 +2687,16 @@
         <v>0</v>
       </c>
       <c r="X61" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="Y61" t="s">
         <v>49</v>
       </c>
       <c r="Z61">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="AA61">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
@@ -2690,16 +2712,16 @@
         <v>0</v>
       </c>
       <c r="X62" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="Y62" t="s">
         <v>49</v>
       </c>
       <c r="Z62">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="AA62">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
@@ -2715,13 +2737,13 @@
         <v>0</v>
       </c>
       <c r="X63" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Y63" t="s">
         <v>49</v>
       </c>
       <c r="Z63">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="AA63">
         <v>2</v>
@@ -2740,13 +2762,13 @@
         <v>0</v>
       </c>
       <c r="X64" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Y64" t="s">
         <v>49</v>
       </c>
       <c r="Z64">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AA64">
         <v>2</v>
@@ -2765,13 +2787,13 @@
         <v>0</v>
       </c>
       <c r="X65" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="Y65" t="s">
         <v>49</v>
       </c>
       <c r="Z65">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="AA65">
         <v>2</v>
@@ -2790,16 +2812,16 @@
         <v>0</v>
       </c>
       <c r="X66" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="Y66" t="s">
         <v>49</v>
       </c>
       <c r="Z66">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="AA66">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
@@ -2815,13 +2837,13 @@
         <v>0</v>
       </c>
       <c r="X67" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Y67" t="s">
         <v>49</v>
       </c>
       <c r="Z67">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="AA67">
         <v>5</v>
@@ -2840,16 +2862,16 @@
         <v>0</v>
       </c>
       <c r="X68" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Y68" t="s">
         <v>49</v>
       </c>
       <c r="Z68">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA68">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
@@ -2865,16 +2887,16 @@
         <v>0</v>
       </c>
       <c r="X69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Y69" t="s">
         <v>49</v>
       </c>
       <c r="Z69">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AA69">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
@@ -2890,16 +2912,16 @@
         <v>0</v>
       </c>
       <c r="X70" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Y70" t="s">
         <v>49</v>
       </c>
       <c r="Z70">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="AA70">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
@@ -2915,16 +2937,16 @@
         <v>0</v>
       </c>
       <c r="X71" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="Y71" t="s">
         <v>49</v>
       </c>
       <c r="Z71">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="AA71">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
@@ -2940,16 +2962,16 @@
         <v>0</v>
       </c>
       <c r="X72" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Y72" t="s">
         <v>49</v>
       </c>
       <c r="Z72">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA72">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
@@ -2965,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="X73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y73" t="s">
         <v>49</v>
@@ -2974,7 +2996,7 @@
         <v>12</v>
       </c>
       <c r="AA73">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
@@ -2990,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="X74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y74" t="s">
         <v>49</v>
@@ -3015,16 +3037,16 @@
         <v>0</v>
       </c>
       <c r="X75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y75" t="s">
         <v>49</v>
       </c>
       <c r="Z75">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA75">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
@@ -3040,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="X76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y76" t="s">
         <v>49</v>
@@ -3049,7 +3071,7 @@
         <v>10</v>
       </c>
       <c r="AA76">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
@@ -3065,16 +3087,16 @@
         <v>0</v>
       </c>
       <c r="X77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Y77" t="s">
         <v>49</v>
       </c>
       <c r="Z77">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="AA77">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
@@ -3090,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="X78" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="Y78" t="s">
         <v>49</v>
@@ -3099,7 +3121,7 @@
         <v>30</v>
       </c>
       <c r="AA78">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
@@ -3115,16 +3137,16 @@
         <v>0</v>
       </c>
       <c r="X79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y79" t="s">
         <v>49</v>
       </c>
       <c r="Z79">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AA79">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
@@ -3140,13 +3162,13 @@
         <v>0</v>
       </c>
       <c r="X80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Y80" t="s">
         <v>49</v>
       </c>
       <c r="Z80">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="AA80">
         <v>2</v>
@@ -3165,16 +3187,16 @@
         <v>0</v>
       </c>
       <c r="X81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y81" t="s">
         <v>49</v>
       </c>
       <c r="Z81">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AA81">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:134" x14ac:dyDescent="0.25">
@@ -3190,16 +3212,16 @@
         <v>0</v>
       </c>
       <c r="X82" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Y82" t="s">
         <v>49</v>
       </c>
       <c r="Z82">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AA82">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:134" x14ac:dyDescent="0.25">
@@ -3215,16 +3237,16 @@
         <v>0</v>
       </c>
       <c r="X83" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Y83" t="s">
         <v>49</v>
       </c>
       <c r="Z83">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AA83">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:134" x14ac:dyDescent="0.25">
@@ -3240,16 +3262,16 @@
         <v>0</v>
       </c>
       <c r="X84" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y84" t="s">
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="Z84">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="AA84">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:134" x14ac:dyDescent="0.25">
@@ -3265,13 +3287,13 @@
         <v>0</v>
       </c>
       <c r="X85" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Y85" t="s">
         <v>145</v>
       </c>
       <c r="Z85">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AA85">
         <v>2</v>
@@ -3290,16 +3312,16 @@
         <v>0</v>
       </c>
       <c r="X86" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Y86" t="s">
         <v>145</v>
       </c>
       <c r="Z86">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="AA86">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:134" x14ac:dyDescent="0.25">
@@ -3315,57 +3337,57 @@
         <v>0</v>
       </c>
       <c r="X87" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="Y87" t="s">
         <v>145</v>
       </c>
       <c r="Z87">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AA87">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:134" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A88" s="36" t="s">
+      <c r="A88" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="B88" s="36"/>
-      <c r="C88" s="36"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="30"/>
       <c r="E88" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F88" s="32" t="s">
+      <c r="F88" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="G88" s="32"/>
-      <c r="H88" s="32"/>
-      <c r="I88" s="32"/>
-      <c r="J88" s="32"/>
-      <c r="K88" s="32"/>
-      <c r="L88" s="32"/>
-      <c r="M88" s="32"/>
-      <c r="N88" s="32"/>
-      <c r="O88" s="32"/>
-      <c r="P88" s="32"/>
-      <c r="Q88" s="32"/>
-      <c r="R88" s="32"/>
-      <c r="S88" s="32"/>
-      <c r="T88" s="32"/>
-      <c r="U88" s="32"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="I88" s="33"/>
+      <c r="J88" s="33"/>
+      <c r="K88" s="33"/>
+      <c r="L88" s="33"/>
+      <c r="M88" s="33"/>
+      <c r="N88" s="33"/>
+      <c r="O88" s="33"/>
+      <c r="P88" s="33"/>
+      <c r="Q88" s="33"/>
+      <c r="R88" s="33"/>
+      <c r="S88" s="33"/>
+      <c r="T88" s="33"/>
+      <c r="U88" s="33"/>
       <c r="X88" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="Y88" t="s">
         <v>145</v>
       </c>
       <c r="Z88">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AA88">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:134" x14ac:dyDescent="0.25">
@@ -3377,33 +3399,33 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F89" s="28"/>
-      <c r="G89" s="28"/>
-      <c r="H89" s="28"/>
-      <c r="I89" s="28"/>
-      <c r="J89" s="28"/>
-      <c r="K89" s="28"/>
-      <c r="L89" s="28"/>
-      <c r="M89" s="28"/>
-      <c r="N89" s="28"/>
-      <c r="O89" s="28"/>
-      <c r="P89" s="28"/>
-      <c r="Q89" s="28"/>
-      <c r="R89" s="28"/>
-      <c r="S89" s="28"/>
-      <c r="T89" s="28"/>
-      <c r="U89" s="28"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="35"/>
+      <c r="H89" s="35"/>
+      <c r="I89" s="35"/>
+      <c r="J89" s="35"/>
+      <c r="K89" s="35"/>
+      <c r="L89" s="35"/>
+      <c r="M89" s="35"/>
+      <c r="N89" s="35"/>
+      <c r="O89" s="35"/>
+      <c r="P89" s="35"/>
+      <c r="Q89" s="35"/>
+      <c r="R89" s="35"/>
+      <c r="S89" s="35"/>
+      <c r="T89" s="35"/>
+      <c r="U89" s="35"/>
       <c r="X89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y89" t="s">
         <v>145</v>
       </c>
       <c r="Z89">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AA89">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:134" x14ac:dyDescent="0.25">
@@ -3418,55 +3440,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F90" s="30" t="str">
+      <c r="F90" s="32" t="str">
         <f>DO90</f>
         <v>Лапки кролика, гредский орех, бутылка</v>
       </c>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="30"/>
-      <c r="L90" s="30"/>
-      <c r="M90" s="30"/>
-      <c r="N90" s="30"/>
-      <c r="O90" s="30"/>
-      <c r="P90" s="30"/>
-      <c r="Q90" s="30"/>
-      <c r="R90" s="30"/>
-      <c r="S90" s="30"/>
-      <c r="T90" s="30"/>
-      <c r="U90" s="30"/>
+      <c r="G90" s="32"/>
+      <c r="H90" s="32"/>
+      <c r="I90" s="32"/>
+      <c r="J90" s="32"/>
+      <c r="K90" s="32"/>
+      <c r="L90" s="32"/>
+      <c r="M90" s="32"/>
+      <c r="N90" s="32"/>
+      <c r="O90" s="32"/>
+      <c r="P90" s="32"/>
+      <c r="Q90" s="32"/>
+      <c r="R90" s="32"/>
+      <c r="S90" s="32"/>
+      <c r="T90" s="32"/>
+      <c r="U90" s="32"/>
       <c r="X90" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y90" t="s">
         <v>145</v>
       </c>
       <c r="Z90">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AA90">
-        <v>3</v>
-      </c>
-      <c r="DO90" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="DO90" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="DP90" s="27"/>
-      <c r="DQ90" s="27"/>
-      <c r="DR90" s="27"/>
-      <c r="DS90" s="27"/>
-      <c r="DT90" s="27"/>
-      <c r="DU90" s="27"/>
-      <c r="DV90" s="27"/>
-      <c r="DW90" s="27"/>
-      <c r="DX90" s="27"/>
-      <c r="DY90" s="27"/>
-      <c r="DZ90" s="27"/>
-      <c r="EA90" s="27"/>
-      <c r="EB90" s="27"/>
-      <c r="EC90" s="27"/>
-      <c r="ED90" s="27"/>
+      <c r="DP90" s="37"/>
+      <c r="DQ90" s="37"/>
+      <c r="DR90" s="37"/>
+      <c r="DS90" s="37"/>
+      <c r="DT90" s="37"/>
+      <c r="DU90" s="37"/>
+      <c r="DV90" s="37"/>
+      <c r="DW90" s="37"/>
+      <c r="DX90" s="37"/>
+      <c r="DY90" s="37"/>
+      <c r="DZ90" s="37"/>
+      <c r="EA90" s="37"/>
+      <c r="EB90" s="37"/>
+      <c r="EC90" s="37"/>
+      <c r="ED90" s="37"/>
     </row>
     <row r="91" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A91" s="16"/>
@@ -3480,55 +3502,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F91" s="30" t="str">
+      <c r="F91" s="32" t="str">
         <f t="shared" ref="F91:F98" si="3">DO91</f>
         <v>Череп(5шт), земля с кладбища, бутылка</v>
       </c>
-      <c r="G91" s="30"/>
-      <c r="H91" s="30"/>
-      <c r="I91" s="30"/>
-      <c r="J91" s="30"/>
-      <c r="K91" s="30"/>
-      <c r="L91" s="30"/>
-      <c r="M91" s="30"/>
-      <c r="N91" s="30"/>
-      <c r="O91" s="30"/>
-      <c r="P91" s="30"/>
-      <c r="Q91" s="30"/>
-      <c r="R91" s="30"/>
-      <c r="S91" s="30"/>
-      <c r="T91" s="30"/>
-      <c r="U91" s="30"/>
+      <c r="G91" s="32"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="32"/>
+      <c r="J91" s="32"/>
+      <c r="K91" s="32"/>
+      <c r="L91" s="32"/>
+      <c r="M91" s="32"/>
+      <c r="N91" s="32"/>
+      <c r="O91" s="32"/>
+      <c r="P91" s="32"/>
+      <c r="Q91" s="32"/>
+      <c r="R91" s="32"/>
+      <c r="S91" s="32"/>
+      <c r="T91" s="32"/>
+      <c r="U91" s="32"/>
       <c r="X91" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="Y91" t="s">
         <v>145</v>
       </c>
       <c r="Z91">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AA91">
-        <v>1</v>
-      </c>
-      <c r="DO91" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="DO91" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="DP91" s="27"/>
-      <c r="DQ91" s="27"/>
-      <c r="DR91" s="27"/>
-      <c r="DS91" s="27"/>
-      <c r="DT91" s="27"/>
-      <c r="DU91" s="27"/>
-      <c r="DV91" s="27"/>
-      <c r="DW91" s="27"/>
-      <c r="DX91" s="27"/>
-      <c r="DY91" s="27"/>
-      <c r="DZ91" s="27"/>
-      <c r="EA91" s="27"/>
-      <c r="EB91" s="27"/>
-      <c r="EC91" s="27"/>
-      <c r="ED91" s="27"/>
+      <c r="DP91" s="37"/>
+      <c r="DQ91" s="37"/>
+      <c r="DR91" s="37"/>
+      <c r="DS91" s="37"/>
+      <c r="DT91" s="37"/>
+      <c r="DU91" s="37"/>
+      <c r="DV91" s="37"/>
+      <c r="DW91" s="37"/>
+      <c r="DX91" s="37"/>
+      <c r="DY91" s="37"/>
+      <c r="DZ91" s="37"/>
+      <c r="EA91" s="37"/>
+      <c r="EB91" s="37"/>
+      <c r="EC91" s="37"/>
+      <c r="ED91" s="37"/>
     </row>
     <row r="92" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A92" s="16"/>
@@ -3542,55 +3564,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F92" s="30" t="str">
+      <c r="F92" s="32" t="str">
         <f t="shared" si="3"/>
         <v>Гредский орехи, череп, сушёные ножки лягушек, голова таракана, слизь, бутылка</v>
       </c>
-      <c r="G92" s="30"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="30"/>
-      <c r="J92" s="30"/>
-      <c r="K92" s="30"/>
-      <c r="L92" s="30"/>
-      <c r="M92" s="30"/>
-      <c r="N92" s="30"/>
-      <c r="O92" s="30"/>
-      <c r="P92" s="30"/>
-      <c r="Q92" s="30"/>
-      <c r="R92" s="30"/>
-      <c r="S92" s="30"/>
-      <c r="T92" s="30"/>
-      <c r="U92" s="30"/>
+      <c r="G92" s="32"/>
+      <c r="H92" s="32"/>
+      <c r="I92" s="32"/>
+      <c r="J92" s="32"/>
+      <c r="K92" s="32"/>
+      <c r="L92" s="32"/>
+      <c r="M92" s="32"/>
+      <c r="N92" s="32"/>
+      <c r="O92" s="32"/>
+      <c r="P92" s="32"/>
+      <c r="Q92" s="32"/>
+      <c r="R92" s="32"/>
+      <c r="S92" s="32"/>
+      <c r="T92" s="32"/>
+      <c r="U92" s="32"/>
       <c r="X92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y92" t="s">
         <v>145</v>
       </c>
       <c r="Z92">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA92">
         <v>1</v>
       </c>
-      <c r="DO92" s="27" t="s">
+      <c r="DO92" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="DP92" s="27"/>
-      <c r="DQ92" s="27"/>
-      <c r="DR92" s="27"/>
-      <c r="DS92" s="27"/>
-      <c r="DT92" s="27"/>
-      <c r="DU92" s="27"/>
-      <c r="DV92" s="27"/>
-      <c r="DW92" s="27"/>
-      <c r="DX92" s="27"/>
-      <c r="DY92" s="27"/>
-      <c r="DZ92" s="27"/>
-      <c r="EA92" s="27"/>
-      <c r="EB92" s="27"/>
-      <c r="EC92" s="27"/>
-      <c r="ED92" s="27"/>
+      <c r="DP92" s="37"/>
+      <c r="DQ92" s="37"/>
+      <c r="DR92" s="37"/>
+      <c r="DS92" s="37"/>
+      <c r="DT92" s="37"/>
+      <c r="DU92" s="37"/>
+      <c r="DV92" s="37"/>
+      <c r="DW92" s="37"/>
+      <c r="DX92" s="37"/>
+      <c r="DY92" s="37"/>
+      <c r="DZ92" s="37"/>
+      <c r="EA92" s="37"/>
+      <c r="EB92" s="37"/>
+      <c r="EC92" s="37"/>
+      <c r="ED92" s="37"/>
     </row>
     <row r="93" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A93" s="16"/>
@@ -3604,55 +3626,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F93" s="30" t="str">
+      <c r="F93" s="32" t="str">
         <f t="shared" si="3"/>
         <v>Гредский орех, череп, мох, бутылка</v>
       </c>
-      <c r="G93" s="30"/>
-      <c r="H93" s="30"/>
-      <c r="I93" s="30"/>
-      <c r="J93" s="30"/>
-      <c r="K93" s="30"/>
-      <c r="L93" s="30"/>
-      <c r="M93" s="30"/>
-      <c r="N93" s="30"/>
-      <c r="O93" s="30"/>
-      <c r="P93" s="30"/>
-      <c r="Q93" s="30"/>
-      <c r="R93" s="30"/>
-      <c r="S93" s="30"/>
-      <c r="T93" s="30"/>
-      <c r="U93" s="30"/>
+      <c r="G93" s="32"/>
+      <c r="H93" s="32"/>
+      <c r="I93" s="32"/>
+      <c r="J93" s="32"/>
+      <c r="K93" s="32"/>
+      <c r="L93" s="32"/>
+      <c r="M93" s="32"/>
+      <c r="N93" s="32"/>
+      <c r="O93" s="32"/>
+      <c r="P93" s="32"/>
+      <c r="Q93" s="32"/>
+      <c r="R93" s="32"/>
+      <c r="S93" s="32"/>
+      <c r="T93" s="32"/>
+      <c r="U93" s="32"/>
       <c r="X93" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="Y93" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z93">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AA93">
         <v>1</v>
       </c>
-      <c r="DO93" s="27" t="s">
+      <c r="DO93" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="DP93" s="27"/>
-      <c r="DQ93" s="27"/>
-      <c r="DR93" s="27"/>
-      <c r="DS93" s="27"/>
-      <c r="DT93" s="27"/>
-      <c r="DU93" s="27"/>
-      <c r="DV93" s="27"/>
-      <c r="DW93" s="27"/>
-      <c r="DX93" s="27"/>
-      <c r="DY93" s="27"/>
-      <c r="DZ93" s="27"/>
-      <c r="EA93" s="27"/>
-      <c r="EB93" s="27"/>
-      <c r="EC93" s="27"/>
-      <c r="ED93" s="27"/>
+      <c r="DP93" s="37"/>
+      <c r="DQ93" s="37"/>
+      <c r="DR93" s="37"/>
+      <c r="DS93" s="37"/>
+      <c r="DT93" s="37"/>
+      <c r="DU93" s="37"/>
+      <c r="DV93" s="37"/>
+      <c r="DW93" s="37"/>
+      <c r="DX93" s="37"/>
+      <c r="DY93" s="37"/>
+      <c r="DZ93" s="37"/>
+      <c r="EA93" s="37"/>
+      <c r="EB93" s="37"/>
+      <c r="EC93" s="37"/>
+      <c r="ED93" s="37"/>
     </row>
     <row r="94" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A94" s="16"/>
@@ -3666,55 +3688,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F94" s="30" t="str">
+      <c r="F94" s="32" t="str">
         <f t="shared" si="3"/>
         <v>Кровь троля, крылья фей(5 шт), бутылка</v>
       </c>
-      <c r="G94" s="30"/>
-      <c r="H94" s="30"/>
-      <c r="I94" s="30"/>
-      <c r="J94" s="30"/>
-      <c r="K94" s="30"/>
-      <c r="L94" s="30"/>
-      <c r="M94" s="30"/>
-      <c r="N94" s="30"/>
-      <c r="O94" s="30"/>
-      <c r="P94" s="30"/>
-      <c r="Q94" s="30"/>
-      <c r="R94" s="30"/>
-      <c r="S94" s="30"/>
-      <c r="T94" s="30"/>
-      <c r="U94" s="30"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="32"/>
+      <c r="J94" s="32"/>
+      <c r="K94" s="32"/>
+      <c r="L94" s="32"/>
+      <c r="M94" s="32"/>
+      <c r="N94" s="32"/>
+      <c r="O94" s="32"/>
+      <c r="P94" s="32"/>
+      <c r="Q94" s="32"/>
+      <c r="R94" s="32"/>
+      <c r="S94" s="32"/>
+      <c r="T94" s="32"/>
+      <c r="U94" s="32"/>
       <c r="X94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Y94" t="s">
         <v>146</v>
       </c>
       <c r="Z94">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AA94">
-        <v>3</v>
-      </c>
-      <c r="DO94" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="DO94" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="DP94" s="27"/>
-      <c r="DQ94" s="27"/>
-      <c r="DR94" s="27"/>
-      <c r="DS94" s="27"/>
-      <c r="DT94" s="27"/>
-      <c r="DU94" s="27"/>
-      <c r="DV94" s="27"/>
-      <c r="DW94" s="27"/>
-      <c r="DX94" s="27"/>
-      <c r="DY94" s="27"/>
-      <c r="DZ94" s="27"/>
-      <c r="EA94" s="27"/>
-      <c r="EB94" s="27"/>
-      <c r="EC94" s="27"/>
-      <c r="ED94" s="27"/>
+      <c r="DP94" s="37"/>
+      <c r="DQ94" s="37"/>
+      <c r="DR94" s="37"/>
+      <c r="DS94" s="37"/>
+      <c r="DT94" s="37"/>
+      <c r="DU94" s="37"/>
+      <c r="DV94" s="37"/>
+      <c r="DW94" s="37"/>
+      <c r="DX94" s="37"/>
+      <c r="DY94" s="37"/>
+      <c r="DZ94" s="37"/>
+      <c r="EA94" s="37"/>
+      <c r="EB94" s="37"/>
+      <c r="EC94" s="37"/>
+      <c r="ED94" s="37"/>
     </row>
     <row r="95" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A95" s="16"/>
@@ -3728,27 +3750,27 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F95" s="30" t="str">
+      <c r="F95" s="32" t="str">
         <f t="shared" si="3"/>
         <v>Мох, шишки, крылья феи(5шт), лист дерева любви, бутылка</v>
       </c>
-      <c r="G95" s="30"/>
-      <c r="H95" s="30"/>
-      <c r="I95" s="30"/>
-      <c r="J95" s="30"/>
-      <c r="K95" s="30"/>
-      <c r="L95" s="30"/>
-      <c r="M95" s="30"/>
-      <c r="N95" s="30"/>
-      <c r="O95" s="30"/>
-      <c r="P95" s="30"/>
-      <c r="Q95" s="30"/>
-      <c r="R95" s="30"/>
-      <c r="S95" s="30"/>
-      <c r="T95" s="30"/>
-      <c r="U95" s="30"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="32"/>
+      <c r="I95" s="32"/>
+      <c r="J95" s="32"/>
+      <c r="K95" s="32"/>
+      <c r="L95" s="32"/>
+      <c r="M95" s="32"/>
+      <c r="N95" s="32"/>
+      <c r="O95" s="32"/>
+      <c r="P95" s="32"/>
+      <c r="Q95" s="32"/>
+      <c r="R95" s="32"/>
+      <c r="S95" s="32"/>
+      <c r="T95" s="32"/>
+      <c r="U95" s="32"/>
       <c r="X95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y95" t="s">
         <v>146</v>
@@ -3757,26 +3779,26 @@
         <v>10</v>
       </c>
       <c r="AA95">
-        <v>2</v>
-      </c>
-      <c r="DO95" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="DO95" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="DP95" s="27"/>
-      <c r="DQ95" s="27"/>
-      <c r="DR95" s="27"/>
-      <c r="DS95" s="27"/>
-      <c r="DT95" s="27"/>
-      <c r="DU95" s="27"/>
-      <c r="DV95" s="27"/>
-      <c r="DW95" s="27"/>
-      <c r="DX95" s="27"/>
-      <c r="DY95" s="27"/>
-      <c r="DZ95" s="27"/>
-      <c r="EA95" s="27"/>
-      <c r="EB95" s="27"/>
-      <c r="EC95" s="27"/>
-      <c r="ED95" s="27"/>
+      <c r="DP95" s="37"/>
+      <c r="DQ95" s="37"/>
+      <c r="DR95" s="37"/>
+      <c r="DS95" s="37"/>
+      <c r="DT95" s="37"/>
+      <c r="DU95" s="37"/>
+      <c r="DV95" s="37"/>
+      <c r="DW95" s="37"/>
+      <c r="DX95" s="37"/>
+      <c r="DY95" s="37"/>
+      <c r="DZ95" s="37"/>
+      <c r="EA95" s="37"/>
+      <c r="EB95" s="37"/>
+      <c r="EC95" s="37"/>
+      <c r="ED95" s="37"/>
     </row>
     <row r="96" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A96" s="16"/>
@@ -3790,55 +3812,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F96" s="30" t="str">
+      <c r="F96" s="32" t="str">
         <f t="shared" si="3"/>
         <v>Лапки кролика, крылья феи, бутылка</v>
       </c>
-      <c r="G96" s="30"/>
-      <c r="H96" s="30"/>
-      <c r="I96" s="30"/>
-      <c r="J96" s="30"/>
-      <c r="K96" s="30"/>
-      <c r="L96" s="30"/>
-      <c r="M96" s="30"/>
-      <c r="N96" s="30"/>
-      <c r="O96" s="30"/>
-      <c r="P96" s="30"/>
-      <c r="Q96" s="30"/>
-      <c r="R96" s="30"/>
-      <c r="S96" s="30"/>
-      <c r="T96" s="30"/>
-      <c r="U96" s="30"/>
+      <c r="G96" s="32"/>
+      <c r="H96" s="32"/>
+      <c r="I96" s="32"/>
+      <c r="J96" s="32"/>
+      <c r="K96" s="32"/>
+      <c r="L96" s="32"/>
+      <c r="M96" s="32"/>
+      <c r="N96" s="32"/>
+      <c r="O96" s="32"/>
+      <c r="P96" s="32"/>
+      <c r="Q96" s="32"/>
+      <c r="R96" s="32"/>
+      <c r="S96" s="32"/>
+      <c r="T96" s="32"/>
+      <c r="U96" s="32"/>
       <c r="X96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y96" t="s">
         <v>146</v>
       </c>
       <c r="Z96">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA96">
-        <v>1</v>
-      </c>
-      <c r="DO96" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="DO96" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="DP96" s="27"/>
-      <c r="DQ96" s="27"/>
-      <c r="DR96" s="27"/>
-      <c r="DS96" s="27"/>
-      <c r="DT96" s="27"/>
-      <c r="DU96" s="27"/>
-      <c r="DV96" s="27"/>
-      <c r="DW96" s="27"/>
-      <c r="DX96" s="27"/>
-      <c r="DY96" s="27"/>
-      <c r="DZ96" s="27"/>
-      <c r="EA96" s="27"/>
-      <c r="EB96" s="27"/>
-      <c r="EC96" s="27"/>
-      <c r="ED96" s="27"/>
+      <c r="DP96" s="37"/>
+      <c r="DQ96" s="37"/>
+      <c r="DR96" s="37"/>
+      <c r="DS96" s="37"/>
+      <c r="DT96" s="37"/>
+      <c r="DU96" s="37"/>
+      <c r="DV96" s="37"/>
+      <c r="DW96" s="37"/>
+      <c r="DX96" s="37"/>
+      <c r="DY96" s="37"/>
+      <c r="DZ96" s="37"/>
+      <c r="EA96" s="37"/>
+      <c r="EB96" s="37"/>
+      <c r="EC96" s="37"/>
+      <c r="ED96" s="37"/>
     </row>
     <row r="97" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A97" s="16"/>
@@ -3852,55 +3874,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F97" s="30" t="str">
+      <c r="F97" s="32" t="str">
         <f t="shared" si="3"/>
         <v>Земля с кладбища, череп, бутылка</v>
       </c>
-      <c r="G97" s="30"/>
-      <c r="H97" s="30"/>
-      <c r="I97" s="30"/>
-      <c r="J97" s="30"/>
-      <c r="K97" s="30"/>
-      <c r="L97" s="30"/>
-      <c r="M97" s="30"/>
-      <c r="N97" s="30"/>
-      <c r="O97" s="30"/>
-      <c r="P97" s="30"/>
-      <c r="Q97" s="30"/>
-      <c r="R97" s="30"/>
-      <c r="S97" s="30"/>
-      <c r="T97" s="30"/>
-      <c r="U97" s="30"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="32"/>
+      <c r="I97" s="32"/>
+      <c r="J97" s="32"/>
+      <c r="K97" s="32"/>
+      <c r="L97" s="32"/>
+      <c r="M97" s="32"/>
+      <c r="N97" s="32"/>
+      <c r="O97" s="32"/>
+      <c r="P97" s="32"/>
+      <c r="Q97" s="32"/>
+      <c r="R97" s="32"/>
+      <c r="S97" s="32"/>
+      <c r="T97" s="32"/>
+      <c r="U97" s="32"/>
       <c r="X97" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="Y97" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Z97">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AA97">
-        <v>25</v>
-      </c>
-      <c r="DO97" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="DO97" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="DP97" s="27"/>
-      <c r="DQ97" s="27"/>
-      <c r="DR97" s="27"/>
-      <c r="DS97" s="27"/>
-      <c r="DT97" s="27"/>
-      <c r="DU97" s="27"/>
-      <c r="DV97" s="27"/>
-      <c r="DW97" s="27"/>
-      <c r="DX97" s="27"/>
-      <c r="DY97" s="27"/>
-      <c r="DZ97" s="27"/>
-      <c r="EA97" s="27"/>
-      <c r="EB97" s="27"/>
-      <c r="EC97" s="27"/>
-      <c r="ED97" s="27"/>
+      <c r="DP97" s="37"/>
+      <c r="DQ97" s="37"/>
+      <c r="DR97" s="37"/>
+      <c r="DS97" s="37"/>
+      <c r="DT97" s="37"/>
+      <c r="DU97" s="37"/>
+      <c r="DV97" s="37"/>
+      <c r="DW97" s="37"/>
+      <c r="DX97" s="37"/>
+      <c r="DY97" s="37"/>
+      <c r="DZ97" s="37"/>
+      <c r="EA97" s="37"/>
+      <c r="EB97" s="37"/>
+      <c r="EC97" s="37"/>
+      <c r="ED97" s="37"/>
     </row>
     <row r="98" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
@@ -3914,55 +3936,55 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F98" s="30" t="str">
+      <c r="F98" s="32" t="str">
         <f t="shared" si="3"/>
         <v>Гредский орехи, сушёные ножки лягушек, голова таракана, слизь, бутылка</v>
       </c>
-      <c r="G98" s="30"/>
-      <c r="H98" s="30"/>
-      <c r="I98" s="30"/>
-      <c r="J98" s="30"/>
-      <c r="K98" s="30"/>
-      <c r="L98" s="30"/>
-      <c r="M98" s="30"/>
-      <c r="N98" s="30"/>
-      <c r="O98" s="30"/>
-      <c r="P98" s="30"/>
-      <c r="Q98" s="30"/>
-      <c r="R98" s="30"/>
-      <c r="S98" s="30"/>
-      <c r="T98" s="30"/>
-      <c r="U98" s="30"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
+      <c r="I98" s="32"/>
+      <c r="J98" s="32"/>
+      <c r="K98" s="32"/>
+      <c r="L98" s="32"/>
+      <c r="M98" s="32"/>
+      <c r="N98" s="32"/>
+      <c r="O98" s="32"/>
+      <c r="P98" s="32"/>
+      <c r="Q98" s="32"/>
+      <c r="R98" s="32"/>
+      <c r="S98" s="32"/>
+      <c r="T98" s="32"/>
+      <c r="U98" s="32"/>
       <c r="X98" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="Y98" t="s">
         <v>147</v>
       </c>
       <c r="Z98">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AA98">
-        <v>21</v>
-      </c>
-      <c r="DO98" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="DO98" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="DP98" s="27"/>
-      <c r="DQ98" s="27"/>
-      <c r="DR98" s="27"/>
-      <c r="DS98" s="27"/>
-      <c r="DT98" s="27"/>
-      <c r="DU98" s="27"/>
-      <c r="DV98" s="27"/>
-      <c r="DW98" s="27"/>
-      <c r="DX98" s="27"/>
-      <c r="DY98" s="27"/>
-      <c r="DZ98" s="27"/>
-      <c r="EA98" s="27"/>
-      <c r="EB98" s="27"/>
-      <c r="EC98" s="27"/>
-      <c r="ED98" s="27"/>
+      <c r="DP98" s="37"/>
+      <c r="DQ98" s="37"/>
+      <c r="DR98" s="37"/>
+      <c r="DS98" s="37"/>
+      <c r="DT98" s="37"/>
+      <c r="DU98" s="37"/>
+      <c r="DV98" s="37"/>
+      <c r="DW98" s="37"/>
+      <c r="DX98" s="37"/>
+      <c r="DY98" s="37"/>
+      <c r="DZ98" s="37"/>
+      <c r="EA98" s="37"/>
+      <c r="EB98" s="37"/>
+      <c r="EC98" s="37"/>
+      <c r="ED98" s="37"/>
     </row>
     <row r="99" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
@@ -3973,33 +3995,33 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F99" s="31"/>
-      <c r="G99" s="31"/>
-      <c r="H99" s="31"/>
-      <c r="I99" s="31"/>
-      <c r="J99" s="31"/>
-      <c r="K99" s="31"/>
-      <c r="L99" s="31"/>
-      <c r="M99" s="31"/>
-      <c r="N99" s="31"/>
-      <c r="O99" s="31"/>
-      <c r="P99" s="31"/>
-      <c r="Q99" s="31"/>
-      <c r="R99" s="31"/>
-      <c r="S99" s="31"/>
-      <c r="T99" s="31"/>
-      <c r="U99" s="31"/>
+      <c r="F99" s="36"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="36"/>
+      <c r="I99" s="36"/>
+      <c r="J99" s="36"/>
+      <c r="K99" s="36"/>
+      <c r="L99" s="36"/>
+      <c r="M99" s="36"/>
+      <c r="N99" s="36"/>
+      <c r="O99" s="36"/>
+      <c r="P99" s="36"/>
+      <c r="Q99" s="36"/>
+      <c r="R99" s="36"/>
+      <c r="S99" s="36"/>
+      <c r="T99" s="36"/>
+      <c r="U99" s="36"/>
       <c r="X99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y99" t="s">
         <v>147</v>
       </c>
       <c r="Z99">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AA99">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:134" x14ac:dyDescent="0.25">
@@ -4014,33 +4036,33 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F100" s="28"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
-      <c r="K100" s="28"/>
-      <c r="L100" s="28"/>
-      <c r="M100" s="28"/>
-      <c r="N100" s="28"/>
-      <c r="O100" s="28"/>
-      <c r="P100" s="28"/>
-      <c r="Q100" s="28"/>
-      <c r="R100" s="28"/>
-      <c r="S100" s="28"/>
-      <c r="T100" s="28"/>
-      <c r="U100" s="28"/>
+      <c r="F100" s="35"/>
+      <c r="G100" s="35"/>
+      <c r="H100" s="35"/>
+      <c r="I100" s="35"/>
+      <c r="J100" s="35"/>
+      <c r="K100" s="35"/>
+      <c r="L100" s="35"/>
+      <c r="M100" s="35"/>
+      <c r="N100" s="35"/>
+      <c r="O100" s="35"/>
+      <c r="P100" s="35"/>
+      <c r="Q100" s="35"/>
+      <c r="R100" s="35"/>
+      <c r="S100" s="35"/>
+      <c r="T100" s="35"/>
+      <c r="U100" s="35"/>
       <c r="X100" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y100" t="s">
         <v>147</v>
       </c>
       <c r="Z100">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA100">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:134" x14ac:dyDescent="0.25">
@@ -4055,30 +4077,30 @@
         <f t="shared" ref="E101:E120" si="4">D101*C101</f>
         <v>0</v>
       </c>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
-      <c r="H101" s="28"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
-      <c r="K101" s="28"/>
-      <c r="L101" s="28"/>
-      <c r="M101" s="28"/>
-      <c r="N101" s="28"/>
-      <c r="O101" s="28"/>
-      <c r="P101" s="28"/>
-      <c r="Q101" s="28"/>
-      <c r="R101" s="28"/>
-      <c r="S101" s="28"/>
-      <c r="T101" s="28"/>
-      <c r="U101" s="28"/>
+      <c r="F101" s="35"/>
+      <c r="G101" s="35"/>
+      <c r="H101" s="35"/>
+      <c r="I101" s="35"/>
+      <c r="J101" s="35"/>
+      <c r="K101" s="35"/>
+      <c r="L101" s="35"/>
+      <c r="M101" s="35"/>
+      <c r="N101" s="35"/>
+      <c r="O101" s="35"/>
+      <c r="P101" s="35"/>
+      <c r="Q101" s="35"/>
+      <c r="R101" s="35"/>
+      <c r="S101" s="35"/>
+      <c r="T101" s="35"/>
+      <c r="U101" s="35"/>
       <c r="X101" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y101" t="s">
         <v>147</v>
       </c>
       <c r="Z101">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="AA101">
         <v>1</v>
@@ -4096,30 +4118,30 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F102" s="28"/>
-      <c r="G102" s="28"/>
-      <c r="H102" s="28"/>
-      <c r="I102" s="28"/>
-      <c r="J102" s="28"/>
-      <c r="K102" s="28"/>
-      <c r="L102" s="28"/>
-      <c r="M102" s="28"/>
-      <c r="N102" s="28"/>
-      <c r="O102" s="28"/>
-      <c r="P102" s="28"/>
-      <c r="Q102" s="28"/>
-      <c r="R102" s="28"/>
-      <c r="S102" s="28"/>
-      <c r="T102" s="28"/>
-      <c r="U102" s="28"/>
+      <c r="F102" s="35"/>
+      <c r="G102" s="35"/>
+      <c r="H102" s="35"/>
+      <c r="I102" s="35"/>
+      <c r="J102" s="35"/>
+      <c r="K102" s="35"/>
+      <c r="L102" s="35"/>
+      <c r="M102" s="35"/>
+      <c r="N102" s="35"/>
+      <c r="O102" s="35"/>
+      <c r="P102" s="35"/>
+      <c r="Q102" s="35"/>
+      <c r="R102" s="35"/>
+      <c r="S102" s="35"/>
+      <c r="T102" s="35"/>
+      <c r="U102" s="35"/>
       <c r="X102" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Y102" t="s">
         <v>147</v>
       </c>
       <c r="Z102">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AA102">
         <v>1</v>
@@ -4137,30 +4159,30 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F103" s="28"/>
-      <c r="G103" s="28"/>
-      <c r="H103" s="28"/>
-      <c r="I103" s="28"/>
-      <c r="J103" s="28"/>
-      <c r="K103" s="28"/>
-      <c r="L103" s="28"/>
-      <c r="M103" s="28"/>
-      <c r="N103" s="28"/>
-      <c r="O103" s="28"/>
-      <c r="P103" s="28"/>
-      <c r="Q103" s="28"/>
-      <c r="R103" s="28"/>
-      <c r="S103" s="28"/>
-      <c r="T103" s="28"/>
-      <c r="U103" s="28"/>
+      <c r="F103" s="35"/>
+      <c r="G103" s="35"/>
+      <c r="H103" s="35"/>
+      <c r="I103" s="35"/>
+      <c r="J103" s="35"/>
+      <c r="K103" s="35"/>
+      <c r="L103" s="35"/>
+      <c r="M103" s="35"/>
+      <c r="N103" s="35"/>
+      <c r="O103" s="35"/>
+      <c r="P103" s="35"/>
+      <c r="Q103" s="35"/>
+      <c r="R103" s="35"/>
+      <c r="S103" s="35"/>
+      <c r="T103" s="35"/>
+      <c r="U103" s="35"/>
       <c r="X103" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y103" t="s">
         <v>147</v>
       </c>
       <c r="Z103">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="AA103">
         <v>1</v>
@@ -4176,30 +4198,30 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F104" s="28"/>
-      <c r="G104" s="28"/>
-      <c r="H104" s="28"/>
-      <c r="I104" s="28"/>
-      <c r="J104" s="28"/>
-      <c r="K104" s="28"/>
-      <c r="L104" s="28"/>
-      <c r="M104" s="28"/>
-      <c r="N104" s="28"/>
-      <c r="O104" s="28"/>
-      <c r="P104" s="28"/>
-      <c r="Q104" s="28"/>
-      <c r="R104" s="28"/>
-      <c r="S104" s="28"/>
-      <c r="T104" s="28"/>
-      <c r="U104" s="28"/>
+      <c r="F104" s="35"/>
+      <c r="G104" s="35"/>
+      <c r="H104" s="35"/>
+      <c r="I104" s="35"/>
+      <c r="J104" s="35"/>
+      <c r="K104" s="35"/>
+      <c r="L104" s="35"/>
+      <c r="M104" s="35"/>
+      <c r="N104" s="35"/>
+      <c r="O104" s="35"/>
+      <c r="P104" s="35"/>
+      <c r="Q104" s="35"/>
+      <c r="R104" s="35"/>
+      <c r="S104" s="35"/>
+      <c r="T104" s="35"/>
+      <c r="U104" s="35"/>
       <c r="X104" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y104" t="s">
         <v>147</v>
       </c>
       <c r="Z104">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="AA104">
         <v>1</v>
@@ -4217,30 +4239,30 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F105" s="28"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="28"/>
-      <c r="I105" s="28"/>
-      <c r="J105" s="28"/>
-      <c r="K105" s="28"/>
-      <c r="L105" s="28"/>
-      <c r="M105" s="28"/>
-      <c r="N105" s="28"/>
-      <c r="O105" s="28"/>
-      <c r="P105" s="28"/>
-      <c r="Q105" s="28"/>
-      <c r="R105" s="28"/>
-      <c r="S105" s="28"/>
-      <c r="T105" s="28"/>
-      <c r="U105" s="28"/>
+      <c r="F105" s="35"/>
+      <c r="G105" s="35"/>
+      <c r="H105" s="35"/>
+      <c r="I105" s="35"/>
+      <c r="J105" s="35"/>
+      <c r="K105" s="35"/>
+      <c r="L105" s="35"/>
+      <c r="M105" s="35"/>
+      <c r="N105" s="35"/>
+      <c r="O105" s="35"/>
+      <c r="P105" s="35"/>
+      <c r="Q105" s="35"/>
+      <c r="R105" s="35"/>
+      <c r="S105" s="35"/>
+      <c r="T105" s="35"/>
+      <c r="U105" s="35"/>
       <c r="X105" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Y105" t="s">
         <v>147</v>
       </c>
       <c r="Z105">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AA105">
         <v>1</v>
@@ -4258,30 +4280,30 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F106" s="28"/>
-      <c r="G106" s="28"/>
-      <c r="H106" s="28"/>
-      <c r="I106" s="28"/>
-      <c r="J106" s="28"/>
-      <c r="K106" s="28"/>
-      <c r="L106" s="28"/>
-      <c r="M106" s="28"/>
-      <c r="N106" s="28"/>
-      <c r="O106" s="28"/>
-      <c r="P106" s="28"/>
-      <c r="Q106" s="28"/>
-      <c r="R106" s="28"/>
-      <c r="S106" s="28"/>
-      <c r="T106" s="28"/>
-      <c r="U106" s="28"/>
+      <c r="F106" s="35"/>
+      <c r="G106" s="35"/>
+      <c r="H106" s="35"/>
+      <c r="I106" s="35"/>
+      <c r="J106" s="35"/>
+      <c r="K106" s="35"/>
+      <c r="L106" s="35"/>
+      <c r="M106" s="35"/>
+      <c r="N106" s="35"/>
+      <c r="O106" s="35"/>
+      <c r="P106" s="35"/>
+      <c r="Q106" s="35"/>
+      <c r="R106" s="35"/>
+      <c r="S106" s="35"/>
+      <c r="T106" s="35"/>
+      <c r="U106" s="35"/>
       <c r="X106" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Y106" t="s">
         <v>147</v>
       </c>
       <c r="Z106">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="AA106">
         <v>1</v>
@@ -4299,30 +4321,30 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F107" s="28"/>
-      <c r="G107" s="28"/>
-      <c r="H107" s="28"/>
-      <c r="I107" s="28"/>
-      <c r="J107" s="28"/>
-      <c r="K107" s="28"/>
-      <c r="L107" s="28"/>
-      <c r="M107" s="28"/>
-      <c r="N107" s="28"/>
-      <c r="O107" s="28"/>
-      <c r="P107" s="28"/>
-      <c r="Q107" s="28"/>
-      <c r="R107" s="28"/>
-      <c r="S107" s="28"/>
-      <c r="T107" s="28"/>
-      <c r="U107" s="28"/>
+      <c r="F107" s="35"/>
+      <c r="G107" s="35"/>
+      <c r="H107" s="35"/>
+      <c r="I107" s="35"/>
+      <c r="J107" s="35"/>
+      <c r="K107" s="35"/>
+      <c r="L107" s="35"/>
+      <c r="M107" s="35"/>
+      <c r="N107" s="35"/>
+      <c r="O107" s="35"/>
+      <c r="P107" s="35"/>
+      <c r="Q107" s="35"/>
+      <c r="R107" s="35"/>
+      <c r="S107" s="35"/>
+      <c r="T107" s="35"/>
+      <c r="U107" s="35"/>
       <c r="X107" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="Y107" t="s">
         <v>147</v>
       </c>
       <c r="Z107">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="AA107">
         <v>1</v>
@@ -4340,32 +4362,32 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F108" s="32" t="s">
+      <c r="F108" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="G108" s="32"/>
-      <c r="H108" s="32"/>
-      <c r="I108" s="32"/>
-      <c r="J108" s="32"/>
-      <c r="K108" s="32"/>
-      <c r="L108" s="32"/>
-      <c r="M108" s="32"/>
-      <c r="N108" s="32"/>
-      <c r="O108" s="32"/>
-      <c r="P108" s="32"/>
-      <c r="Q108" s="32"/>
-      <c r="R108" s="32"/>
-      <c r="S108" s="32"/>
-      <c r="T108" s="32"/>
-      <c r="U108" s="32"/>
+      <c r="G108" s="33"/>
+      <c r="H108" s="33"/>
+      <c r="I108" s="33"/>
+      <c r="J108" s="33"/>
+      <c r="K108" s="33"/>
+      <c r="L108" s="33"/>
+      <c r="M108" s="33"/>
+      <c r="N108" s="33"/>
+      <c r="O108" s="33"/>
+      <c r="P108" s="33"/>
+      <c r="Q108" s="33"/>
+      <c r="R108" s="33"/>
+      <c r="S108" s="33"/>
+      <c r="T108" s="33"/>
+      <c r="U108" s="33"/>
       <c r="X108" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="Y108" t="s">
         <v>147</v>
       </c>
       <c r="Z108">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AA108">
         <v>1</v>
@@ -4383,55 +4405,55 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F109" s="29" t="str">
+      <c r="F109" s="31" t="str">
         <f>DO109</f>
         <v>"Вода тавой друг, но не на долго(20 минут раздвигаешь воду)"</v>
       </c>
-      <c r="G109" s="29"/>
-      <c r="H109" s="29"/>
-      <c r="I109" s="29"/>
-      <c r="J109" s="29"/>
-      <c r="K109" s="29"/>
-      <c r="L109" s="29"/>
-      <c r="M109" s="29"/>
-      <c r="N109" s="29"/>
-      <c r="O109" s="29"/>
-      <c r="P109" s="29"/>
-      <c r="Q109" s="29"/>
-      <c r="R109" s="29"/>
-      <c r="S109" s="29"/>
-      <c r="T109" s="29"/>
-      <c r="U109" s="29"/>
+      <c r="G109" s="31"/>
+      <c r="H109" s="31"/>
+      <c r="I109" s="31"/>
+      <c r="J109" s="31"/>
+      <c r="K109" s="31"/>
+      <c r="L109" s="31"/>
+      <c r="M109" s="31"/>
+      <c r="N109" s="31"/>
+      <c r="O109" s="31"/>
+      <c r="P109" s="31"/>
+      <c r="Q109" s="31"/>
+      <c r="R109" s="31"/>
+      <c r="S109" s="31"/>
+      <c r="T109" s="31"/>
+      <c r="U109" s="31"/>
       <c r="X109" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="Y109" t="s">
         <v>147</v>
       </c>
       <c r="Z109">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AA109">
         <v>1</v>
       </c>
-      <c r="DO109" s="29" t="s">
+      <c r="DO109" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="DP109" s="29"/>
-      <c r="DQ109" s="29"/>
-      <c r="DR109" s="29"/>
-      <c r="DS109" s="29"/>
-      <c r="DT109" s="29"/>
-      <c r="DU109" s="29"/>
-      <c r="DV109" s="29"/>
-      <c r="DW109" s="29"/>
-      <c r="DX109" s="29"/>
-      <c r="DY109" s="29"/>
-      <c r="DZ109" s="29"/>
-      <c r="EA109" s="29"/>
-      <c r="EB109" s="29"/>
-      <c r="EC109" s="29"/>
-      <c r="ED109" s="29"/>
+      <c r="DP109" s="31"/>
+      <c r="DQ109" s="31"/>
+      <c r="DR109" s="31"/>
+      <c r="DS109" s="31"/>
+      <c r="DT109" s="31"/>
+      <c r="DU109" s="31"/>
+      <c r="DV109" s="31"/>
+      <c r="DW109" s="31"/>
+      <c r="DX109" s="31"/>
+      <c r="DY109" s="31"/>
+      <c r="DZ109" s="31"/>
+      <c r="EA109" s="31"/>
+      <c r="EB109" s="31"/>
+      <c r="EC109" s="31"/>
+      <c r="ED109" s="31"/>
     </row>
     <row r="110" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
@@ -4445,55 +4467,55 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F110" s="29" t="str">
+      <c r="F110" s="31" t="str">
         <f t="shared" ref="F110:F117" si="5">DO110</f>
         <v>"Могут принимать любую внешности и надев их человек будет танцевать до сильнйо сталости - снять может только другой человек"</v>
       </c>
-      <c r="G110" s="29"/>
-      <c r="H110" s="29"/>
-      <c r="I110" s="29"/>
-      <c r="J110" s="29"/>
-      <c r="K110" s="29"/>
-      <c r="L110" s="29"/>
-      <c r="M110" s="29"/>
-      <c r="N110" s="29"/>
-      <c r="O110" s="29"/>
-      <c r="P110" s="29"/>
-      <c r="Q110" s="29"/>
-      <c r="R110" s="29"/>
-      <c r="S110" s="29"/>
-      <c r="T110" s="29"/>
-      <c r="U110" s="29"/>
+      <c r="G110" s="31"/>
+      <c r="H110" s="31"/>
+      <c r="I110" s="31"/>
+      <c r="J110" s="31"/>
+      <c r="K110" s="31"/>
+      <c r="L110" s="31"/>
+      <c r="M110" s="31"/>
+      <c r="N110" s="31"/>
+      <c r="O110" s="31"/>
+      <c r="P110" s="31"/>
+      <c r="Q110" s="31"/>
+      <c r="R110" s="31"/>
+      <c r="S110" s="31"/>
+      <c r="T110" s="31"/>
+      <c r="U110" s="31"/>
       <c r="X110" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="Y110" t="s">
         <v>147</v>
       </c>
       <c r="Z110">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="AA110">
-        <v>2</v>
-      </c>
-      <c r="DO110" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="DO110" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="DP110" s="29"/>
-      <c r="DQ110" s="29"/>
-      <c r="DR110" s="29"/>
-      <c r="DS110" s="29"/>
-      <c r="DT110" s="29"/>
-      <c r="DU110" s="29"/>
-      <c r="DV110" s="29"/>
-      <c r="DW110" s="29"/>
-      <c r="DX110" s="29"/>
-      <c r="DY110" s="29"/>
-      <c r="DZ110" s="29"/>
-      <c r="EA110" s="29"/>
-      <c r="EB110" s="29"/>
-      <c r="EC110" s="29"/>
-      <c r="ED110" s="29"/>
+      <c r="DP110" s="31"/>
+      <c r="DQ110" s="31"/>
+      <c r="DR110" s="31"/>
+      <c r="DS110" s="31"/>
+      <c r="DT110" s="31"/>
+      <c r="DU110" s="31"/>
+      <c r="DV110" s="31"/>
+      <c r="DW110" s="31"/>
+      <c r="DX110" s="31"/>
+      <c r="DY110" s="31"/>
+      <c r="DZ110" s="31"/>
+      <c r="EA110" s="31"/>
+      <c r="EB110" s="31"/>
+      <c r="EC110" s="31"/>
+      <c r="ED110" s="31"/>
     </row>
     <row r="111" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
@@ -4507,55 +4529,55 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F111" s="29" t="str">
+      <c r="F111" s="31" t="str">
         <f t="shared" si="5"/>
         <v>"Взглянув в него человек вспоминает самое худшее в его жизни - будь с этим осторожны"</v>
       </c>
-      <c r="G111" s="29"/>
-      <c r="H111" s="29"/>
-      <c r="I111" s="29"/>
-      <c r="J111" s="29"/>
-      <c r="K111" s="29"/>
-      <c r="L111" s="29"/>
-      <c r="M111" s="29"/>
-      <c r="N111" s="29"/>
-      <c r="O111" s="29"/>
-      <c r="P111" s="29"/>
-      <c r="Q111" s="29"/>
-      <c r="R111" s="29"/>
-      <c r="S111" s="29"/>
-      <c r="T111" s="29"/>
-      <c r="U111" s="29"/>
+      <c r="G111" s="31"/>
+      <c r="H111" s="31"/>
+      <c r="I111" s="31"/>
+      <c r="J111" s="31"/>
+      <c r="K111" s="31"/>
+      <c r="L111" s="31"/>
+      <c r="M111" s="31"/>
+      <c r="N111" s="31"/>
+      <c r="O111" s="31"/>
+      <c r="P111" s="31"/>
+      <c r="Q111" s="31"/>
+      <c r="R111" s="31"/>
+      <c r="S111" s="31"/>
+      <c r="T111" s="31"/>
+      <c r="U111" s="31"/>
       <c r="X111" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="Y111" t="s">
         <v>147</v>
       </c>
       <c r="Z111">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AA111">
-        <v>6</v>
-      </c>
-      <c r="DO111" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="DO111" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="DP111" s="29"/>
-      <c r="DQ111" s="29"/>
-      <c r="DR111" s="29"/>
-      <c r="DS111" s="29"/>
-      <c r="DT111" s="29"/>
-      <c r="DU111" s="29"/>
-      <c r="DV111" s="29"/>
-      <c r="DW111" s="29"/>
-      <c r="DX111" s="29"/>
-      <c r="DY111" s="29"/>
-      <c r="DZ111" s="29"/>
-      <c r="EA111" s="29"/>
-      <c r="EB111" s="29"/>
-      <c r="EC111" s="29"/>
-      <c r="ED111" s="29"/>
+      <c r="DP111" s="31"/>
+      <c r="DQ111" s="31"/>
+      <c r="DR111" s="31"/>
+      <c r="DS111" s="31"/>
+      <c r="DT111" s="31"/>
+      <c r="DU111" s="31"/>
+      <c r="DV111" s="31"/>
+      <c r="DW111" s="31"/>
+      <c r="DX111" s="31"/>
+      <c r="DY111" s="31"/>
+      <c r="DZ111" s="31"/>
+      <c r="EA111" s="31"/>
+      <c r="EB111" s="31"/>
+      <c r="EC111" s="31"/>
+      <c r="ED111" s="31"/>
     </row>
     <row r="112" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
@@ -4569,55 +4591,55 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F112" s="29" t="str">
+      <c r="F112" s="31" t="str">
         <f t="shared" si="5"/>
         <v>"Меняет погоду один раз на 1 час положив на него частичку погоды - лист, вода, песок и т д"</v>
       </c>
-      <c r="G112" s="29"/>
-      <c r="H112" s="29"/>
-      <c r="I112" s="29"/>
-      <c r="J112" s="29"/>
-      <c r="K112" s="29"/>
-      <c r="L112" s="29"/>
-      <c r="M112" s="29"/>
-      <c r="N112" s="29"/>
-      <c r="O112" s="29"/>
-      <c r="P112" s="29"/>
-      <c r="Q112" s="29"/>
-      <c r="R112" s="29"/>
-      <c r="S112" s="29"/>
-      <c r="T112" s="29"/>
-      <c r="U112" s="29"/>
+      <c r="G112" s="31"/>
+      <c r="H112" s="31"/>
+      <c r="I112" s="31"/>
+      <c r="J112" s="31"/>
+      <c r="K112" s="31"/>
+      <c r="L112" s="31"/>
+      <c r="M112" s="31"/>
+      <c r="N112" s="31"/>
+      <c r="O112" s="31"/>
+      <c r="P112" s="31"/>
+      <c r="Q112" s="31"/>
+      <c r="R112" s="31"/>
+      <c r="S112" s="31"/>
+      <c r="T112" s="31"/>
+      <c r="U112" s="31"/>
       <c r="X112" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y112" t="s">
         <v>147</v>
       </c>
       <c r="Z112">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AA112">
-        <v>3</v>
-      </c>
-      <c r="DO112" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="DO112" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="DP112" s="29"/>
-      <c r="DQ112" s="29"/>
-      <c r="DR112" s="29"/>
-      <c r="DS112" s="29"/>
-      <c r="DT112" s="29"/>
-      <c r="DU112" s="29"/>
-      <c r="DV112" s="29"/>
-      <c r="DW112" s="29"/>
-      <c r="DX112" s="29"/>
-      <c r="DY112" s="29"/>
-      <c r="DZ112" s="29"/>
-      <c r="EA112" s="29"/>
-      <c r="EB112" s="29"/>
-      <c r="EC112" s="29"/>
-      <c r="ED112" s="29"/>
+      <c r="DP112" s="31"/>
+      <c r="DQ112" s="31"/>
+      <c r="DR112" s="31"/>
+      <c r="DS112" s="31"/>
+      <c r="DT112" s="31"/>
+      <c r="DU112" s="31"/>
+      <c r="DV112" s="31"/>
+      <c r="DW112" s="31"/>
+      <c r="DX112" s="31"/>
+      <c r="DY112" s="31"/>
+      <c r="DZ112" s="31"/>
+      <c r="EA112" s="31"/>
+      <c r="EB112" s="31"/>
+      <c r="EC112" s="31"/>
+      <c r="ED112" s="31"/>
     </row>
     <row r="113" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
@@ -4631,43 +4653,55 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F113" s="29" t="str">
+      <c r="F113" s="31" t="str">
         <f t="shared" si="5"/>
         <v>"Уничтожает свет и поджигает то, на что у огня нет сил"</v>
       </c>
-      <c r="G113" s="29"/>
-      <c r="H113" s="29"/>
-      <c r="I113" s="29"/>
-      <c r="J113" s="29"/>
-      <c r="K113" s="29"/>
-      <c r="L113" s="29"/>
-      <c r="M113" s="29"/>
-      <c r="N113" s="29"/>
-      <c r="O113" s="29"/>
-      <c r="P113" s="29"/>
-      <c r="Q113" s="29"/>
-      <c r="R113" s="29"/>
-      <c r="S113" s="29"/>
-      <c r="T113" s="29"/>
-      <c r="U113" s="29"/>
-      <c r="DO113" s="29" t="s">
+      <c r="G113" s="31"/>
+      <c r="H113" s="31"/>
+      <c r="I113" s="31"/>
+      <c r="J113" s="31"/>
+      <c r="K113" s="31"/>
+      <c r="L113" s="31"/>
+      <c r="M113" s="31"/>
+      <c r="N113" s="31"/>
+      <c r="O113" s="31"/>
+      <c r="P113" s="31"/>
+      <c r="Q113" s="31"/>
+      <c r="R113" s="31"/>
+      <c r="S113" s="31"/>
+      <c r="T113" s="31"/>
+      <c r="U113" s="31"/>
+      <c r="X113" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y113" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z113">
+        <v>9</v>
+      </c>
+      <c r="AA113">
+        <v>3</v>
+      </c>
+      <c r="DO113" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="DP113" s="29"/>
-      <c r="DQ113" s="29"/>
-      <c r="DR113" s="29"/>
-      <c r="DS113" s="29"/>
-      <c r="DT113" s="29"/>
-      <c r="DU113" s="29"/>
-      <c r="DV113" s="29"/>
-      <c r="DW113" s="29"/>
-      <c r="DX113" s="29"/>
-      <c r="DY113" s="29"/>
-      <c r="DZ113" s="29"/>
-      <c r="EA113" s="29"/>
-      <c r="EB113" s="29"/>
-      <c r="EC113" s="29"/>
-      <c r="ED113" s="29"/>
+      <c r="DP113" s="31"/>
+      <c r="DQ113" s="31"/>
+      <c r="DR113" s="31"/>
+      <c r="DS113" s="31"/>
+      <c r="DT113" s="31"/>
+      <c r="DU113" s="31"/>
+      <c r="DV113" s="31"/>
+      <c r="DW113" s="31"/>
+      <c r="DX113" s="31"/>
+      <c r="DY113" s="31"/>
+      <c r="DZ113" s="31"/>
+      <c r="EA113" s="31"/>
+      <c r="EB113" s="31"/>
+      <c r="EC113" s="31"/>
+      <c r="ED113" s="31"/>
     </row>
     <row r="114" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
@@ -4681,43 +4715,43 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F114" s="29" t="str">
+      <c r="F114" s="31" t="str">
         <f t="shared" si="5"/>
         <v>"Призывает маленькую фею с эффектом природы - даёт свет, дыхание под водой на 10 минут, отгоняет демонов - но её силы ограничены"</v>
       </c>
-      <c r="G114" s="29"/>
-      <c r="H114" s="29"/>
-      <c r="I114" s="29"/>
-      <c r="J114" s="29"/>
-      <c r="K114" s="29"/>
-      <c r="L114" s="29"/>
-      <c r="M114" s="29"/>
-      <c r="N114" s="29"/>
-      <c r="O114" s="29"/>
-      <c r="P114" s="29"/>
-      <c r="Q114" s="29"/>
-      <c r="R114" s="29"/>
-      <c r="S114" s="29"/>
-      <c r="T114" s="29"/>
-      <c r="U114" s="29"/>
-      <c r="DO114" s="29" t="s">
+      <c r="G114" s="31"/>
+      <c r="H114" s="31"/>
+      <c r="I114" s="31"/>
+      <c r="J114" s="31"/>
+      <c r="K114" s="31"/>
+      <c r="L114" s="31"/>
+      <c r="M114" s="31"/>
+      <c r="N114" s="31"/>
+      <c r="O114" s="31"/>
+      <c r="P114" s="31"/>
+      <c r="Q114" s="31"/>
+      <c r="R114" s="31"/>
+      <c r="S114" s="31"/>
+      <c r="T114" s="31"/>
+      <c r="U114" s="31"/>
+      <c r="DO114" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="DP114" s="29"/>
-      <c r="DQ114" s="29"/>
-      <c r="DR114" s="29"/>
-      <c r="DS114" s="29"/>
-      <c r="DT114" s="29"/>
-      <c r="DU114" s="29"/>
-      <c r="DV114" s="29"/>
-      <c r="DW114" s="29"/>
-      <c r="DX114" s="29"/>
-      <c r="DY114" s="29"/>
-      <c r="DZ114" s="29"/>
-      <c r="EA114" s="29"/>
-      <c r="EB114" s="29"/>
-      <c r="EC114" s="29"/>
-      <c r="ED114" s="29"/>
+      <c r="DP114" s="31"/>
+      <c r="DQ114" s="31"/>
+      <c r="DR114" s="31"/>
+      <c r="DS114" s="31"/>
+      <c r="DT114" s="31"/>
+      <c r="DU114" s="31"/>
+      <c r="DV114" s="31"/>
+      <c r="DW114" s="31"/>
+      <c r="DX114" s="31"/>
+      <c r="DY114" s="31"/>
+      <c r="DZ114" s="31"/>
+      <c r="EA114" s="31"/>
+      <c r="EB114" s="31"/>
+      <c r="EC114" s="31"/>
+      <c r="ED114" s="31"/>
     </row>
     <row r="115" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
@@ -4731,43 +4765,43 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F115" s="29" t="str">
+      <c r="F115" s="31" t="str">
         <f t="shared" si="5"/>
         <v>"Заклинает игрока или нпс и делает из него крысу на 10 минут (не работает на боссов)"</v>
       </c>
-      <c r="G115" s="29"/>
-      <c r="H115" s="29"/>
-      <c r="I115" s="29"/>
-      <c r="J115" s="29"/>
-      <c r="K115" s="29"/>
-      <c r="L115" s="29"/>
-      <c r="M115" s="29"/>
-      <c r="N115" s="29"/>
-      <c r="O115" s="29"/>
-      <c r="P115" s="29"/>
-      <c r="Q115" s="29"/>
-      <c r="R115" s="29"/>
-      <c r="S115" s="29"/>
-      <c r="T115" s="29"/>
-      <c r="U115" s="29"/>
-      <c r="DO115" s="29" t="s">
+      <c r="G115" s="31"/>
+      <c r="H115" s="31"/>
+      <c r="I115" s="31"/>
+      <c r="J115" s="31"/>
+      <c r="K115" s="31"/>
+      <c r="L115" s="31"/>
+      <c r="M115" s="31"/>
+      <c r="N115" s="31"/>
+      <c r="O115" s="31"/>
+      <c r="P115" s="31"/>
+      <c r="Q115" s="31"/>
+      <c r="R115" s="31"/>
+      <c r="S115" s="31"/>
+      <c r="T115" s="31"/>
+      <c r="U115" s="31"/>
+      <c r="DO115" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="DP115" s="29"/>
-      <c r="DQ115" s="29"/>
-      <c r="DR115" s="29"/>
-      <c r="DS115" s="29"/>
-      <c r="DT115" s="29"/>
-      <c r="DU115" s="29"/>
-      <c r="DV115" s="29"/>
-      <c r="DW115" s="29"/>
-      <c r="DX115" s="29"/>
-      <c r="DY115" s="29"/>
-      <c r="DZ115" s="29"/>
-      <c r="EA115" s="29"/>
-      <c r="EB115" s="29"/>
-      <c r="EC115" s="29"/>
-      <c r="ED115" s="29"/>
+      <c r="DP115" s="31"/>
+      <c r="DQ115" s="31"/>
+      <c r="DR115" s="31"/>
+      <c r="DS115" s="31"/>
+      <c r="DT115" s="31"/>
+      <c r="DU115" s="31"/>
+      <c r="DV115" s="31"/>
+      <c r="DW115" s="31"/>
+      <c r="DX115" s="31"/>
+      <c r="DY115" s="31"/>
+      <c r="DZ115" s="31"/>
+      <c r="EA115" s="31"/>
+      <c r="EB115" s="31"/>
+      <c r="EC115" s="31"/>
+      <c r="ED115" s="31"/>
     </row>
     <row r="116" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
@@ -4781,43 +4815,43 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F116" s="29" t="str">
+      <c r="F116" s="31" t="str">
         <f t="shared" si="5"/>
         <v>"Убирает память до младенчества (на игроков не работает) - направленный"</v>
       </c>
-      <c r="G116" s="29"/>
-      <c r="H116" s="29"/>
-      <c r="I116" s="29"/>
-      <c r="J116" s="29"/>
-      <c r="K116" s="29"/>
-      <c r="L116" s="29"/>
-      <c r="M116" s="29"/>
-      <c r="N116" s="29"/>
-      <c r="O116" s="29"/>
-      <c r="P116" s="29"/>
-      <c r="Q116" s="29"/>
-      <c r="R116" s="29"/>
-      <c r="S116" s="29"/>
-      <c r="T116" s="29"/>
-      <c r="U116" s="29"/>
-      <c r="DO116" s="29" t="s">
+      <c r="G116" s="31"/>
+      <c r="H116" s="31"/>
+      <c r="I116" s="31"/>
+      <c r="J116" s="31"/>
+      <c r="K116" s="31"/>
+      <c r="L116" s="31"/>
+      <c r="M116" s="31"/>
+      <c r="N116" s="31"/>
+      <c r="O116" s="31"/>
+      <c r="P116" s="31"/>
+      <c r="Q116" s="31"/>
+      <c r="R116" s="31"/>
+      <c r="S116" s="31"/>
+      <c r="T116" s="31"/>
+      <c r="U116" s="31"/>
+      <c r="DO116" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="DP116" s="29"/>
-      <c r="DQ116" s="29"/>
-      <c r="DR116" s="29"/>
-      <c r="DS116" s="29"/>
-      <c r="DT116" s="29"/>
-      <c r="DU116" s="29"/>
-      <c r="DV116" s="29"/>
-      <c r="DW116" s="29"/>
-      <c r="DX116" s="29"/>
-      <c r="DY116" s="29"/>
-      <c r="DZ116" s="29"/>
-      <c r="EA116" s="29"/>
-      <c r="EB116" s="29"/>
-      <c r="EC116" s="29"/>
-      <c r="ED116" s="29"/>
+      <c r="DP116" s="31"/>
+      <c r="DQ116" s="31"/>
+      <c r="DR116" s="31"/>
+      <c r="DS116" s="31"/>
+      <c r="DT116" s="31"/>
+      <c r="DU116" s="31"/>
+      <c r="DV116" s="31"/>
+      <c r="DW116" s="31"/>
+      <c r="DX116" s="31"/>
+      <c r="DY116" s="31"/>
+      <c r="DZ116" s="31"/>
+      <c r="EA116" s="31"/>
+      <c r="EB116" s="31"/>
+      <c r="EC116" s="31"/>
+      <c r="ED116" s="31"/>
     </row>
     <row r="117" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
@@ -4831,43 +4865,43 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F117" s="29" t="str">
+      <c r="F117" s="31" t="str">
         <f t="shared" si="5"/>
         <v>"Призывает 1 огромную(и правда большую) змею с ядом на 10 минут (2 раунда)- 100 урона 50 хп"</v>
       </c>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
-      <c r="L117" s="29"/>
-      <c r="M117" s="29"/>
-      <c r="N117" s="29"/>
-      <c r="O117" s="29"/>
-      <c r="P117" s="29"/>
-      <c r="Q117" s="29"/>
-      <c r="R117" s="29"/>
-      <c r="S117" s="29"/>
-      <c r="T117" s="29"/>
-      <c r="U117" s="29"/>
-      <c r="DO117" s="29" t="s">
+      <c r="G117" s="31"/>
+      <c r="H117" s="31"/>
+      <c r="I117" s="31"/>
+      <c r="J117" s="31"/>
+      <c r="K117" s="31"/>
+      <c r="L117" s="31"/>
+      <c r="M117" s="31"/>
+      <c r="N117" s="31"/>
+      <c r="O117" s="31"/>
+      <c r="P117" s="31"/>
+      <c r="Q117" s="31"/>
+      <c r="R117" s="31"/>
+      <c r="S117" s="31"/>
+      <c r="T117" s="31"/>
+      <c r="U117" s="31"/>
+      <c r="DO117" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="DP117" s="29"/>
-      <c r="DQ117" s="29"/>
-      <c r="DR117" s="29"/>
-      <c r="DS117" s="29"/>
-      <c r="DT117" s="29"/>
-      <c r="DU117" s="29"/>
-      <c r="DV117" s="29"/>
-      <c r="DW117" s="29"/>
-      <c r="DX117" s="29"/>
-      <c r="DY117" s="29"/>
-      <c r="DZ117" s="29"/>
-      <c r="EA117" s="29"/>
-      <c r="EB117" s="29"/>
-      <c r="EC117" s="29"/>
-      <c r="ED117" s="29"/>
+      <c r="DP117" s="31"/>
+      <c r="DQ117" s="31"/>
+      <c r="DR117" s="31"/>
+      <c r="DS117" s="31"/>
+      <c r="DT117" s="31"/>
+      <c r="DU117" s="31"/>
+      <c r="DV117" s="31"/>
+      <c r="DW117" s="31"/>
+      <c r="DX117" s="31"/>
+      <c r="DY117" s="31"/>
+      <c r="DZ117" s="31"/>
+      <c r="EA117" s="31"/>
+      <c r="EB117" s="31"/>
+      <c r="EC117" s="31"/>
+      <c r="ED117" s="31"/>
     </row>
     <row r="118" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
@@ -4881,22 +4915,22 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F118" s="28"/>
-      <c r="G118" s="28"/>
-      <c r="H118" s="28"/>
-      <c r="I118" s="28"/>
-      <c r="J118" s="28"/>
-      <c r="K118" s="28"/>
-      <c r="L118" s="28"/>
-      <c r="M118" s="28"/>
-      <c r="N118" s="28"/>
-      <c r="O118" s="28"/>
-      <c r="P118" s="28"/>
-      <c r="Q118" s="28"/>
-      <c r="R118" s="28"/>
-      <c r="S118" s="28"/>
-      <c r="T118" s="28"/>
-      <c r="U118" s="28"/>
+      <c r="F118" s="35"/>
+      <c r="G118" s="35"/>
+      <c r="H118" s="35"/>
+      <c r="I118" s="35"/>
+      <c r="J118" s="35"/>
+      <c r="K118" s="35"/>
+      <c r="L118" s="35"/>
+      <c r="M118" s="35"/>
+      <c r="N118" s="35"/>
+      <c r="O118" s="35"/>
+      <c r="P118" s="35"/>
+      <c r="Q118" s="35"/>
+      <c r="R118" s="35"/>
+      <c r="S118" s="35"/>
+      <c r="T118" s="35"/>
+      <c r="U118" s="35"/>
     </row>
     <row r="119" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
@@ -4910,22 +4944,22 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F119" s="28"/>
-      <c r="G119" s="28"/>
-      <c r="H119" s="28"/>
-      <c r="I119" s="28"/>
-      <c r="J119" s="28"/>
-      <c r="K119" s="28"/>
-      <c r="L119" s="28"/>
-      <c r="M119" s="28"/>
-      <c r="N119" s="28"/>
-      <c r="O119" s="28"/>
-      <c r="P119" s="28"/>
-      <c r="Q119" s="28"/>
-      <c r="R119" s="28"/>
-      <c r="S119" s="28"/>
-      <c r="T119" s="28"/>
-      <c r="U119" s="28"/>
+      <c r="F119" s="35"/>
+      <c r="G119" s="35"/>
+      <c r="H119" s="35"/>
+      <c r="I119" s="35"/>
+      <c r="J119" s="35"/>
+      <c r="K119" s="35"/>
+      <c r="L119" s="35"/>
+      <c r="M119" s="35"/>
+      <c r="N119" s="35"/>
+      <c r="O119" s="35"/>
+      <c r="P119" s="35"/>
+      <c r="Q119" s="35"/>
+      <c r="R119" s="35"/>
+      <c r="S119" s="35"/>
+      <c r="T119" s="35"/>
+      <c r="U119" s="35"/>
     </row>
     <row r="120" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
@@ -4939,36 +4973,54 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F120" s="28"/>
-      <c r="G120" s="28"/>
-      <c r="H120" s="28"/>
-      <c r="I120" s="28"/>
-      <c r="J120" s="28"/>
-      <c r="K120" s="28"/>
-      <c r="L120" s="28"/>
-      <c r="M120" s="28"/>
-      <c r="N120" s="28"/>
-      <c r="O120" s="28"/>
-      <c r="P120" s="28"/>
-      <c r="Q120" s="28"/>
-      <c r="R120" s="28"/>
-      <c r="S120" s="28"/>
-      <c r="T120" s="28"/>
-      <c r="U120" s="28"/>
+      <c r="F120" s="35"/>
+      <c r="G120" s="35"/>
+      <c r="H120" s="35"/>
+      <c r="I120" s="35"/>
+      <c r="J120" s="35"/>
+      <c r="K120" s="35"/>
+      <c r="L120" s="35"/>
+      <c r="M120" s="35"/>
+      <c r="N120" s="35"/>
+      <c r="O120" s="35"/>
+      <c r="P120" s="35"/>
+      <c r="Q120" s="35"/>
+      <c r="R120" s="35"/>
+      <c r="S120" s="35"/>
+      <c r="T120" s="35"/>
+      <c r="U120" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="F109:U109"/>
-    <mergeCell ref="F94:U94"/>
-    <mergeCell ref="F95:U95"/>
-    <mergeCell ref="F96:U96"/>
-    <mergeCell ref="F97:U97"/>
-    <mergeCell ref="F88:U88"/>
-    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="DO95:ED95"/>
+    <mergeCell ref="F104:U104"/>
+    <mergeCell ref="F105:U105"/>
+    <mergeCell ref="F106:U106"/>
+    <mergeCell ref="F107:U107"/>
+    <mergeCell ref="DO90:ED90"/>
+    <mergeCell ref="DO91:ED91"/>
+    <mergeCell ref="DO92:ED92"/>
+    <mergeCell ref="DO93:ED93"/>
+    <mergeCell ref="DO94:ED94"/>
+    <mergeCell ref="DO115:ED115"/>
+    <mergeCell ref="DO116:ED116"/>
+    <mergeCell ref="DO117:ED117"/>
+    <mergeCell ref="DO96:ED96"/>
+    <mergeCell ref="DO97:ED97"/>
+    <mergeCell ref="DO98:ED98"/>
+    <mergeCell ref="DO109:ED109"/>
+    <mergeCell ref="DO110:ED110"/>
+    <mergeCell ref="DO111:ED111"/>
+    <mergeCell ref="DO112:ED112"/>
+    <mergeCell ref="DO113:ED113"/>
+    <mergeCell ref="DO114:ED114"/>
+    <mergeCell ref="F119:U119"/>
+    <mergeCell ref="F98:U98"/>
+    <mergeCell ref="F99:U99"/>
+    <mergeCell ref="F100:U100"/>
+    <mergeCell ref="F101:U101"/>
+    <mergeCell ref="F102:U102"/>
+    <mergeCell ref="F108:U108"/>
     <mergeCell ref="F120:U120"/>
     <mergeCell ref="F89:U89"/>
     <mergeCell ref="F90:U90"/>
@@ -4985,35 +5037,17 @@
     <mergeCell ref="F116:U116"/>
     <mergeCell ref="F117:U117"/>
     <mergeCell ref="F118:U118"/>
-    <mergeCell ref="F119:U119"/>
-    <mergeCell ref="F98:U98"/>
-    <mergeCell ref="F99:U99"/>
-    <mergeCell ref="F100:U100"/>
-    <mergeCell ref="F101:U101"/>
-    <mergeCell ref="F102:U102"/>
-    <mergeCell ref="F108:U108"/>
-    <mergeCell ref="DO115:ED115"/>
-    <mergeCell ref="DO116:ED116"/>
-    <mergeCell ref="DO117:ED117"/>
-    <mergeCell ref="DO96:ED96"/>
-    <mergeCell ref="DO97:ED97"/>
-    <mergeCell ref="DO98:ED98"/>
-    <mergeCell ref="DO109:ED109"/>
-    <mergeCell ref="DO110:ED110"/>
-    <mergeCell ref="DO111:ED111"/>
-    <mergeCell ref="DO112:ED112"/>
-    <mergeCell ref="DO113:ED113"/>
-    <mergeCell ref="DO114:ED114"/>
-    <mergeCell ref="DO90:ED90"/>
-    <mergeCell ref="DO91:ED91"/>
-    <mergeCell ref="DO92:ED92"/>
-    <mergeCell ref="DO93:ED93"/>
-    <mergeCell ref="DO94:ED94"/>
-    <mergeCell ref="DO95:ED95"/>
-    <mergeCell ref="F104:U104"/>
-    <mergeCell ref="F105:U105"/>
-    <mergeCell ref="F106:U106"/>
-    <mergeCell ref="F107:U107"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="F109:U109"/>
+    <mergeCell ref="F94:U94"/>
+    <mergeCell ref="F95:U95"/>
+    <mergeCell ref="F96:U96"/>
+    <mergeCell ref="F97:U97"/>
+    <mergeCell ref="F88:U88"/>
+    <mergeCell ref="I2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>